<commit_message>
fix bug, add test result, add readme
</commit_message>
<xml_diff>
--- a/TestCase.xlsx
+++ b/TestCase.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2503" uniqueCount="811">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4086" uniqueCount="847">
   <si>
     <t>Module</t>
   </si>
@@ -3760,6 +3760,121 @@
   </si>
   <si>
     <t>Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.xpath: //a[contains(@href,"suppoting</t>
+  </si>
+  <si>
+    <t>B01_LoginWithInvalidCredential.jpg</t>
+  </si>
+  <si>
+    <t>B02_LoginWithUnverifiedUserAccount.jpg</t>
+  </si>
+  <si>
+    <t>H01_GettingStarted.jpg</t>
+  </si>
+  <si>
+    <t>H02_MerchantOnBoarding.jpg</t>
+  </si>
+  <si>
+    <t>J01_FirstStepAddService.jpg</t>
+  </si>
+  <si>
+    <t>J02_SecondStepService.jpg</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.id: service_step_two' (tried for 10 second(s) with 500 MILLISECONDS interval)</t>
+  </si>
+  <si>
+    <t>C03_ForgetPasswordWithValidEmailCredential.jpg</t>
+  </si>
+  <si>
+    <t>G02_DownloadFile.jpg</t>
+  </si>
+  <si>
+    <t>J04_FourthStepService.jpg</t>
+  </si>
+  <si>
+    <t>K01_AccessListServicePage.jpg</t>
+  </si>
+  <si>
+    <t>K02_ActivateService.jpg</t>
+  </si>
+  <si>
+    <t>K03_DeactiveService.jpg</t>
+  </si>
+  <si>
+    <t>K05_EditServiceWithAllMandatoryFieldsAreFilled.jpg</t>
+  </si>
+  <si>
+    <t>N03_InviteUserWithValidCredential.jpg</t>
+  </si>
+  <si>
+    <t>O01_ClickOnApproveButtonRejectButtonWithoutSelectCheckbox.jpg</t>
+  </si>
+  <si>
+    <t>O02_RejectUser.jpg</t>
+  </si>
+  <si>
+    <t>O02_ApproveUser.jpg</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//td[2 and contains(text(),"yopmail")]/../td/div/input"}
+  (Session info: headless chrome=88.0.4324.150)
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.14.0', revision: 'aacccce0', time: '2018</t>
+  </si>
+  <si>
+    <t>R02_SearchServiceManagement.jpg</t>
+  </si>
+  <si>
+    <t>R04_RejectService.jpg</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.xpath: //tr//td[8 and (contains(text(),"Approved") or contains(text(),"Submitted"))]/../td/a[@class="btn color</t>
+  </si>
+  <si>
+    <t>K04_EditServiceWithLetOneOrAllMandatoryFieldsAreEmpty.jpg</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//tr/td[8]/../td[@class="text</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.xpath: //a[@href="/list</t>
+  </si>
+  <si>
+    <t>R03_ApproveService.jpg</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//*[contains(text(),"src0347")]/../td/a[@class="btn btn</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//*[contains(text(),"src0348")]/../td/a[@class="btn btn</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.xpath: //button[contains(text(),"reject")]' (tried for 10 second(s) with 500 MILLISECONDS interval)</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"xpath","selector":"//button[contains(text(),"reject")]"}
+  (Session info: chrome=88.0.4324.150)
+For documentation on this error, please visit: http://seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.14.0', revision: 'aacccce0', time: '2018</t>
+  </si>
+  <si>
+    <t>The following asserts failed:
+	message is not displayed did not expect to find [true] but found [false]</t>
+  </si>
+  <si>
+    <t>F03_UpdatePasswordWithCorrectInput.jpg</t>
+  </si>
+  <si>
+    <t>J03_ThirdStepService.jpg</t>
+  </si>
+  <si>
+    <t>N01_InviteUserWithAllMandatoryAreEmpty.jpg</t>
+  </si>
+  <si>
+    <t>N02_InviteTakenUsernameOrTakenEmailAddress.jpg</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of Proxy element for: DefaultElementLocator 'By.id: username' (tried for 10 second(s) with 500 MILLISECONDS interval)</t>
   </si>
 </sst>
 </file>
@@ -4942,7 +5057,7 @@
         <v>729</v>
       </c>
       <c r="J3" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K3" s="98" t="s">
         <v>12</v>
@@ -4977,7 +5092,7 @@
         <v>740</v>
       </c>
       <c r="J4" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K4" s="98" t="s">
         <v>12</v>
@@ -5012,7 +5127,7 @@
         <v>740</v>
       </c>
       <c r="J5" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K5" s="98" t="s">
         <v>12</v>
@@ -5047,7 +5162,7 @@
         <v>740</v>
       </c>
       <c r="J6" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K6" s="98" t="s">
         <v>12</v>
@@ -5080,7 +5195,7 @@
         <v>802</v>
       </c>
       <c r="J7" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K7" s="98" t="s">
         <v>12</v>
@@ -5113,7 +5228,7 @@
         <v>739</v>
       </c>
       <c r="J8" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K8" s="98" t="s">
         <v>12</v>
@@ -5199,7 +5314,7 @@
         <v>729</v>
       </c>
       <c r="J11" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K11" s="98" t="s">
         <v>12</v>
@@ -5232,7 +5347,7 @@
         <v>729</v>
       </c>
       <c r="J12" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K12" s="98" t="s">
         <v>12</v>
@@ -5265,7 +5380,7 @@
         <v>729</v>
       </c>
       <c r="J13" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K13" s="98" t="s">
         <v>12</v>
@@ -5318,7 +5433,7 @@
         <v>729</v>
       </c>
       <c r="J15" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K15" s="98" t="s">
         <v>12</v>
@@ -5353,7 +5468,7 @@
         <v>729</v>
       </c>
       <c r="J16" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K16" s="98" t="s">
         <v>12</v>
@@ -5386,7 +5501,7 @@
         <v>729</v>
       </c>
       <c r="J17" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K17" s="98" t="s">
         <v>12</v>
@@ -5529,10 +5644,10 @@
         <v>729</v>
       </c>
       <c r="J22" s="98" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="K22" s="98" t="s">
-        <v>808</v>
+        <v>12</v>
       </c>
       <c r="L22" s="98" t="s">
         <v>12</v>
@@ -5562,13 +5677,13 @@
         <v>729</v>
       </c>
       <c r="J23" s="98" t="s">
-        <v>805</v>
+        <v>801</v>
       </c>
       <c r="K23" s="98" t="s">
-        <v>806</v>
+        <v>12</v>
       </c>
       <c r="L23" s="98" t="s">
-        <v>810</v>
+        <v>12</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="70" x14ac:dyDescent="0.15">
@@ -5595,7 +5710,7 @@
         <v>729</v>
       </c>
       <c r="J24" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K24" s="98" t="s">
         <v>12</v>
@@ -5628,7 +5743,7 @@
         <v>729</v>
       </c>
       <c r="J25" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K25" s="98" t="s">
         <v>12</v>
@@ -5661,7 +5776,7 @@
         <v>803</v>
       </c>
       <c r="J26" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K26" s="98" t="s">
         <v>12</v>
@@ -5716,7 +5831,7 @@
         <v>729</v>
       </c>
       <c r="J28" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K28" s="98" t="s">
         <v>12</v>
@@ -5749,7 +5864,7 @@
         <v>729</v>
       </c>
       <c r="J29" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K29" s="98" t="s">
         <v>12</v>
@@ -5782,10 +5897,10 @@
         <v>729</v>
       </c>
       <c r="J30" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K30" s="98" t="s">
-        <v>12</v>
+        <v>842</v>
       </c>
       <c r="L30" s="98" t="s">
         <v>12</v>
@@ -5837,7 +5952,7 @@
         <v>729</v>
       </c>
       <c r="J32" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K32" s="98" t="s">
         <v>12</v>
@@ -5870,10 +5985,10 @@
         <v>729</v>
       </c>
       <c r="J33" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K33" s="98" t="s">
-        <v>12</v>
+        <v>819</v>
       </c>
       <c r="L33" s="98" t="s">
         <v>12</v>
@@ -5925,7 +6040,7 @@
         <v>740</v>
       </c>
       <c r="J35" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K35" s="98" t="s">
         <v>12</v>
@@ -5959,7 +6074,7 @@
         <v>740</v>
       </c>
       <c r="J36" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K36" s="98" t="s">
         <v>12</v>
@@ -5993,7 +6108,7 @@
         <v>740</v>
       </c>
       <c r="J37" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K37" s="98" t="s">
         <v>12</v>
@@ -6027,7 +6142,7 @@
         <v>740</v>
       </c>
       <c r="J38" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K38" s="98" t="s">
         <v>12</v>
@@ -6061,7 +6176,7 @@
         <v>740</v>
       </c>
       <c r="J39" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K39" s="98" t="s">
         <v>12</v>
@@ -6095,7 +6210,7 @@
         <v>740</v>
       </c>
       <c r="J40" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K40" s="98" t="s">
         <v>12</v>
@@ -6205,10 +6320,10 @@
         <v>729</v>
       </c>
       <c r="J44" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K44" s="98" t="s">
-        <v>12</v>
+        <v>815</v>
       </c>
       <c r="L44" s="98" t="s">
         <v>12</v>
@@ -6238,10 +6353,10 @@
         <v>729</v>
       </c>
       <c r="J45" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K45" s="98" t="s">
-        <v>12</v>
+        <v>816</v>
       </c>
       <c r="L45" s="98" t="s">
         <v>12</v>
@@ -6271,10 +6386,10 @@
         <v>729</v>
       </c>
       <c r="J46" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K46" s="98" t="s">
-        <v>12</v>
+        <v>843</v>
       </c>
       <c r="L46" s="98" t="s">
         <v>12</v>
@@ -6304,10 +6419,10 @@
         <v>729</v>
       </c>
       <c r="J47" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K47" s="98" t="s">
-        <v>12</v>
+        <v>820</v>
       </c>
       <c r="L47" s="98" t="s">
         <v>12</v>
@@ -6337,7 +6452,7 @@
         <v>729</v>
       </c>
       <c r="J48" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K48" s="98" t="s">
         <v>12</v>
@@ -6370,7 +6485,7 @@
         <v>729</v>
       </c>
       <c r="J49" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K49" s="98" t="s">
         <v>12</v>
@@ -6425,10 +6540,10 @@
         <v>729</v>
       </c>
       <c r="J51" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K51" s="98" t="s">
-        <v>12</v>
+        <v>821</v>
       </c>
       <c r="L51" s="98" t="s">
         <v>12</v>
@@ -6490,10 +6605,10 @@
         <v>740</v>
       </c>
       <c r="J53" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K53" s="98" t="s">
-        <v>12</v>
+        <v>822</v>
       </c>
       <c r="L53" s="98" t="s">
         <v>12</v>
@@ -6523,10 +6638,10 @@
         <v>740</v>
       </c>
       <c r="J54" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K54" s="98" t="s">
-        <v>12</v>
+        <v>823</v>
       </c>
       <c r="L54" s="98" t="s">
         <v>12</v>
@@ -6556,7 +6671,7 @@
         <v>740</v>
       </c>
       <c r="J55" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K55" s="98" t="s">
         <v>12</v>
@@ -6589,13 +6704,13 @@
         <v>740</v>
       </c>
       <c r="J56" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K56" s="98" t="s">
-        <v>12</v>
+        <v>824</v>
       </c>
       <c r="L56" s="98" t="s">
-        <v>12</v>
+        <v>838</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -7120,10 +7235,10 @@
         <v>729</v>
       </c>
       <c r="J73" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K73" s="98" t="s">
-        <v>12</v>
+        <v>844</v>
       </c>
       <c r="L73" s="98" t="s">
         <v>12</v>
@@ -7153,10 +7268,10 @@
         <v>740</v>
       </c>
       <c r="J74" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K74" s="98" t="s">
-        <v>12</v>
+        <v>845</v>
       </c>
       <c r="L74" s="98" t="s">
         <v>12</v>
@@ -7186,13 +7301,13 @@
         <v>740</v>
       </c>
       <c r="J75" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K75" s="98" t="s">
-        <v>12</v>
+        <v>825</v>
       </c>
       <c r="L75" s="98" t="s">
-        <v>12</v>
+        <v>846</v>
       </c>
     </row>
     <row r="76" spans="1:12" ht="13" x14ac:dyDescent="0.15">
@@ -7241,7 +7356,7 @@
         <v>740</v>
       </c>
       <c r="J77" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K77" s="98" t="s">
         <v>12</v>
@@ -7274,13 +7389,13 @@
         <v>740</v>
       </c>
       <c r="J78" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K78" s="98" t="s">
-        <v>12</v>
+        <v>827</v>
       </c>
       <c r="L78" s="98" t="s">
-        <v>12</v>
+        <v>841</v>
       </c>
     </row>
     <row r="79" spans="1:12" ht="70" x14ac:dyDescent="0.15">
@@ -7307,7 +7422,7 @@
         <v>740</v>
       </c>
       <c r="J79" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K79" s="98" t="s">
         <v>12</v>
@@ -7736,7 +7851,7 @@
         <v>729</v>
       </c>
       <c r="J93" s="97" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K93" s="98" t="s">
         <v>12</v>
@@ -7769,7 +7884,7 @@
         <v>729</v>
       </c>
       <c r="J94" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K94" s="98" t="s">
         <v>12</v>
@@ -7802,7 +7917,7 @@
         <v>729</v>
       </c>
       <c r="J95" s="98" t="s">
-        <v>12</v>
+        <v>801</v>
       </c>
       <c r="K95" s="98" t="s">
         <v>12</v>
@@ -7835,13 +7950,13 @@
         <v>729</v>
       </c>
       <c r="J96" s="98" t="s">
-        <v>12</v>
+        <v>805</v>
       </c>
       <c r="K96" s="98" t="s">
-        <v>12</v>
+        <v>831</v>
       </c>
       <c r="L96" s="98" t="s">
-        <v>12</v>
+        <v>832</v>
       </c>
     </row>
     <row r="97" spans="1:27" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>